<commit_message>
perbaikan brian 26 januari 2025
</commit_message>
<xml_diff>
--- a/assets/file_format_import/format_barang_toko_gudang_import.xlsx
+++ b/assets/file_format_import/format_barang_toko_gudang_import.xlsx
@@ -1,45 +1,62 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\sinargantari\assets\file_format_import\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\sinargantari\assets\file_format_import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED06CE3-8A0C-4CBC-B88D-1B6EAA3AF319}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5B599F09-899C-4430-99E3-570D05DE903F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{005CA784-F360-4100-A9FA-ED294600A87E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{15725BB7-1A61-4675-BC8D-1A0C0D920FEC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>status</t>
-  </si>
-  <si>
-    <t>nama_barang</t>
-  </si>
-  <si>
-    <t>nama_gudang</t>
-  </si>
-  <si>
-    <t>jumlah_barang</t>
-  </si>
-  <si>
-    <t>nama_toko_luar</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>Nama Barang</t>
+  </si>
+  <si>
+    <t>Nama Gudang</t>
+  </si>
+  <si>
+    <t>Jumlah Barang</t>
+  </si>
+  <si>
+    <t>Nama Toko Luar</t>
+  </si>
+  <si>
+    <t>Travo 5A O</t>
+  </si>
+  <si>
+    <t>Sumber Agung Gudang</t>
+  </si>
+  <si>
+    <t>Shopee</t>
   </si>
 </sst>
 </file>
@@ -50,9 +67,8 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
-      <charset val="1"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -113,39 +129,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="E97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="196B24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -197,7 +213,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -308,13 +324,6 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -323,6 +332,13 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -387,27 +403,53 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B37CE6B-4AFE-401C-B0B9-35B34663DC88}">
-  <dimension ref="A1:E1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0375A92-A980-4F62-A26A-3F8805685973}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -420,8 +462,19 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>